<commit_message>
Updated package and help button
</commit_message>
<xml_diff>
--- a/Client_Logs.xlsx
+++ b/Client_Logs.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet name="Sheet1" sheetId="1" state="visible" r:id="R305c1dbb70f74eebab448f2ea1ff9e94"/>
+    <x:sheet name="Sheet1" sheetId="1" state="visible" r:id="Rbba1b06637114f70bbb0826e34fde8a7"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -117,7 +117,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:dimension ref="A1:J2"/>
+  <x:dimension ref="A1:J3"/>
   <x:sheetViews>
     <x:sheetView tabSelected="0" workbookViewId="0">
       <x:pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -163,7 +163,7 @@
         <x:v>Any Photo</x:v>
       </x:c>
       <x:c r="I1" t="str" s="1">
-        <x:v>instax</x:v>
+        <x:v>Solo/Group</x:v>
       </x:c>
       <x:c r="J1" t="str" s="1">
         <x:v>TimeStamp</x:v>
@@ -201,8 +201,40 @@
         <x:v>2025-12-14 13:13:03</x:v>
       </x:c>
     </x:row>
+    <x:row r="3">
+      <x:c r="A3" t="str" s="2">
+        <x:v>DONE CHOOSING</x:v>
+      </x:c>
+      <x:c r="B3" t="str" s="2">
+        <x:v>ASD</x:v>
+      </x:c>
+      <x:c r="C3" t="str" s="2">
+        <x:v>asd@asd.asd</x:v>
+      </x:c>
+      <x:c r="D3" t="str" s="2">
+        <x:v>Basic</x:v>
+      </x:c>
+      <x:c r="E3" t="str" s="2">
+        <x:v>ABOGADO, MAISA C.jpeg</x:v>
+      </x:c>
+      <x:c r="F3" t="str" s="2">
+        <x:v>N/A</x:v>
+      </x:c>
+      <x:c r="G3" t="str" s="2">
+        <x:v>N/A</x:v>
+      </x:c>
+      <x:c r="H3" t="str" s="2">
+        <x:v>N/A</x:v>
+      </x:c>
+      <x:c r="I3" t="str" s="2">
+        <x:v>N/A</x:v>
+      </x:c>
+      <x:c r="J3" t="str" s="2">
+        <x:v>2026-01-16 00:51:24</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
-  <x:autoFilter ref="A1:J2"/>
+  <x:autoFilter ref="A1:J3"/>
   <x:drawing r:id="drawing1"/>
 </x:worksheet>
 </file>
</xml_diff>